<commit_message>
Pega in class project - signing in and ordering prduct
</commit_message>
<xml_diff>
--- a/Week2/StringMan_RegEx/SuperHero_SpreadSheet.xlsx
+++ b/Week2/StringMan_RegEx/SuperHero_SpreadSheet.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <x:workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Michael-Rometty-230206\Week2\StringMan_RegEx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5916" firstSheet="0" activeTab="0"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="Super" sheetId="1" r:id="rId1"/>
-  </x:sheets>
-  <x:definedNames/>
-  <x:calcPr calcId="152511"/>
-  <x:extLst>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5916"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Super" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="152511"/>
+  <extLst>
     <x:ext xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -28,108 +27,62 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </x:ext>
-  </x:extLst>
-</x:workbook>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <x:si>
-    <x:t>Name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Identity</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Location</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Superman</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Clark Kent</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Fortress of Solitude</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Batman</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Bruce Wayne</x:t>
-  </x:si>
-  <x:si>
-    <x:t>The Batcave</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Wonderwoman</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Diana</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Themyscira</x:t>
-  </x:si>
-</x:sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <x:numFmts count="1">
-    <x:numFmt numFmtId="0" formatCode=""/>
-  </x:numFmts>
-  <x:fonts count="2" x14ac:knownFonts="1">
-    <x:font>
-      <x:sz val="11"/>
-      <x:color theme="1"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-      <x:scheme val="minor"/>
-    </x:font>
-    <x:font>
-      <x:vertAlign val="baseline"/>
-      <x:sz val="11"/>
-      <x:color rgb="FF000000"/>
-      <x:name val="Calibri"/>
-      <x:family val="2"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </x:cellStyleXfs>
-  <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
-</x:styleSheet>
+    </ext>
+  </extLst>
+</styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,72 +381,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <x:sheetPr>
-    <x:outlinePr summaryBelow="1" summaryRight="1"/>
-  </x:sheetPr>
-  <x:dimension ref="A1:C4"/>
-  <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="B5" sqref="B5"/>
-    </x:sheetView>
-  </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <x:cols>
-    <x:col min="1" max="1" width="19.441406" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="21.777344" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="29.554688" style="0" customWidth="1"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <x:c r="A1" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <x:c r="A2" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <x:c r="A3" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <x:c r="A4" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
-  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
-  <x:headerFooter/>
-  <x:tableParts count="0"/>
-</x:worksheet>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>